<commit_message>
Eliminacion de tareas no planeadad en lista de tareas
</commit_message>
<xml_diff>
--- a/Lista de tareas individuales/Lista_Tareas_Revision_3_-_David_Barcenas_Duran.xlsx
+++ b/Lista de tareas individuales/Lista_Tareas_Revision_3_-_David_Barcenas_Duran.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bestr\Desktop\Repositorios\ItaliaPizza-doc\Lista de tareas individuales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C561F29-B5B9-425B-B69F-096724661C3E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6D8219E-9177-46A0-9020-2D0DBEA5AAC7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14424" yWindow="2760" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Casos de Uso" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="90">
   <si>
     <t>Columna</t>
   </si>
@@ -301,6 +301,15 @@
   </si>
   <si>
     <t>DBD, JAGL, GSC</t>
+  </si>
+  <si>
+    <t>Finalizado</t>
+  </si>
+  <si>
+    <t>Terminado</t>
+  </si>
+  <si>
+    <t>Duda</t>
   </si>
 </sst>
 </file>
@@ -833,18 +842,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:BA26"/>
+  <dimension ref="A1:BA25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane xSplit="6" ySplit="5" topLeftCell="AL18" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="5" topLeftCell="AB6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="E25" sqref="E25"/>
+      <selection pane="bottomRight" activeCell="A23" sqref="A23:XFD23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="1.44140625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="15.44140625" style="2" customWidth="1"/>
     <col min="2" max="2" width="16.44140625" style="2" customWidth="1"/>
     <col min="3" max="3" width="34" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.77734375" style="2" bestFit="1" customWidth="1"/>
@@ -900,15 +909,15 @@
     <col min="54" max="16384" width="10.77734375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:53" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:53" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="B1" s="12" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="2:53" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:53" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" s="12"/>
     </row>
-    <row r="3" spans="2:53" ht="21" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:53" ht="21" x14ac:dyDescent="0.4">
       <c r="B3" s="3" t="s">
         <v>28</v>
       </c>
@@ -916,7 +925,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="2:53" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:53" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H4" s="17" t="s">
         <v>5</v>
       </c>
@@ -996,7 +1005,7 @@
       </c>
       <c r="BA4" s="18"/>
     </row>
-    <row r="5" spans="2:53" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:53" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B5" s="6" t="s">
         <v>27</v>
       </c>
@@ -1126,7 +1135,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="2:53" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:53" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B6" s="13" t="s">
         <v>47</v>
       </c>
@@ -1140,7 +1149,7 @@
         <v>54</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="G6" s="5">
         <v>4</v>
@@ -1240,7 +1249,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="2:53" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:53" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B7" s="13"/>
       <c r="C7" s="5"/>
       <c r="D7" s="16" t="s">
@@ -1350,7 +1359,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="2:53" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:53" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B8" s="13" t="s">
         <v>48</v>
       </c>
@@ -1364,7 +1373,7 @@
         <v>54</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="G8" s="5">
         <v>4</v>
@@ -1464,7 +1473,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="2:53" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:53" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B9" s="13" t="s">
         <v>49</v>
       </c>
@@ -1485,100 +1494,100 @@
       </c>
       <c r="H9" s="8"/>
       <c r="I9" s="8">
-        <f t="shared" ref="I9:I23" si="32">G9-H9</f>
+        <f t="shared" ref="I9:I22" si="32">G9-H9</f>
         <v>4</v>
       </c>
       <c r="J9" s="10"/>
       <c r="K9" s="8"/>
       <c r="L9" s="8">
-        <f t="shared" ref="L9:L23" si="33">I9-K9</f>
+        <f t="shared" ref="L9:L22" si="33">I9-K9</f>
         <v>4</v>
       </c>
       <c r="M9" s="10"/>
       <c r="N9" s="8"/>
       <c r="O9" s="8">
-        <f t="shared" ref="O9:O23" si="34">L9-N9</f>
+        <f t="shared" ref="O9:O22" si="34">L9-N9</f>
         <v>4</v>
       </c>
       <c r="P9" s="10"/>
       <c r="Q9" s="8"/>
       <c r="R9" s="8">
-        <f t="shared" ref="R9:R23" si="35">O9-Q9</f>
+        <f t="shared" ref="R9:R22" si="35">O9-Q9</f>
         <v>4</v>
       </c>
       <c r="S9" s="10"/>
       <c r="T9" s="8"/>
       <c r="U9" s="8">
-        <f t="shared" ref="U9:U23" si="36">R9-T9</f>
+        <f t="shared" ref="U9:U22" si="36">R9-T9</f>
         <v>4</v>
       </c>
       <c r="V9" s="10"/>
       <c r="W9" s="8"/>
       <c r="X9" s="8">
-        <f t="shared" ref="X9:X23" si="37">U9-W9</f>
+        <f t="shared" ref="X9:X22" si="37">U9-W9</f>
         <v>4</v>
       </c>
       <c r="Y9" s="10"/>
       <c r="Z9" s="8"/>
       <c r="AA9" s="8">
-        <f t="shared" ref="AA9:AA23" si="38">X9-Z9</f>
+        <f t="shared" ref="AA9:AA22" si="38">X9-Z9</f>
         <v>4</v>
       </c>
       <c r="AB9" s="10"/>
       <c r="AC9" s="8"/>
       <c r="AD9" s="8">
-        <f t="shared" ref="AD9:AD23" si="39">AA9-AC9</f>
+        <f t="shared" ref="AD9:AD22" si="39">AA9-AC9</f>
         <v>4</v>
       </c>
       <c r="AE9" s="10"/>
       <c r="AF9" s="8"/>
       <c r="AG9" s="8">
-        <f t="shared" ref="AG9:AG23" si="40">AD9-AF9</f>
+        <f t="shared" ref="AG9:AG22" si="40">AD9-AF9</f>
         <v>4</v>
       </c>
       <c r="AH9" s="10"/>
       <c r="AI9" s="8"/>
       <c r="AJ9" s="8">
-        <f t="shared" ref="AJ9:AJ23" si="41">AG9-AI9</f>
+        <f t="shared" ref="AJ9:AJ22" si="41">AG9-AI9</f>
         <v>4</v>
       </c>
       <c r="AK9" s="10"/>
       <c r="AL9" s="8"/>
       <c r="AM9" s="8">
-        <f t="shared" ref="AM9:AM23" si="42">AJ9-AL9</f>
+        <f t="shared" ref="AM9:AM22" si="42">AJ9-AL9</f>
         <v>4</v>
       </c>
       <c r="AN9" s="10"/>
       <c r="AO9" s="8"/>
       <c r="AP9" s="8">
-        <f t="shared" ref="AP9:AP23" si="43">AM9-AO9</f>
+        <f t="shared" ref="AP9:AP22" si="43">AM9-AO9</f>
         <v>4</v>
       </c>
       <c r="AQ9" s="10"/>
       <c r="AR9" s="8"/>
       <c r="AS9" s="8">
-        <f t="shared" ref="AS9:AS23" si="44">AP9-AR9</f>
+        <f t="shared" ref="AS9:AS22" si="44">AP9-AR9</f>
         <v>4</v>
       </c>
       <c r="AT9" s="10"/>
       <c r="AU9" s="8"/>
       <c r="AV9" s="8">
-        <f t="shared" ref="AV9:AV23" si="45">AS9-AU9</f>
+        <f t="shared" ref="AV9:AV22" si="45">AS9-AU9</f>
         <v>4</v>
       </c>
       <c r="AW9" s="10"/>
       <c r="AX9" s="8"/>
       <c r="AY9" s="8">
-        <f t="shared" ref="AY9:AY23" si="46">AV9-AX9</f>
+        <f t="shared" ref="AY9:AY22" si="46">AV9-AX9</f>
         <v>4</v>
       </c>
       <c r="AZ9" s="15"/>
       <c r="BA9" s="11">
-        <f t="shared" ref="BA9:BA23" si="47">G9-AZ9</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="2:53" ht="43.2" x14ac:dyDescent="0.3">
+        <f t="shared" ref="BA9:BA22" si="47">G9-AZ9</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:53" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B10" s="13"/>
       <c r="C10" s="5"/>
       <c r="D10" s="16" t="s">
@@ -1688,7 +1697,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="2:53" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:53" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B11" s="13" t="s">
         <v>50</v>
       </c>
@@ -1702,7 +1711,7 @@
         <v>54</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G11" s="5">
         <v>4</v>
@@ -1802,7 +1811,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="2:53" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:53" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B12" s="13"/>
       <c r="C12" s="5"/>
       <c r="D12" s="16" t="s">
@@ -1812,7 +1821,7 @@
         <v>54</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G12" s="5">
         <v>4</v>
@@ -1912,7 +1921,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="2:53" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:53" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>89</v>
+      </c>
       <c r="B13" s="13" t="s">
         <v>51</v>
       </c>
@@ -2026,7 +2038,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="2:53" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:53" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B14" s="13"/>
       <c r="C14" s="5"/>
       <c r="D14" s="16" t="s">
@@ -2136,7 +2148,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="2:53" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:53" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B15" s="13" t="s">
         <v>52</v>
       </c>
@@ -2150,7 +2162,7 @@
         <v>54</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="G15" s="5">
         <v>4</v>
@@ -2250,7 +2262,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="2:53" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:53" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B16" s="13"/>
       <c r="C16" s="5"/>
       <c r="D16" s="16" t="s">
@@ -2260,7 +2272,7 @@
         <v>54</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G16" s="5">
         <v>4</v>
@@ -2368,7 +2380,7 @@
         <v>76</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>54</v>
@@ -2381,107 +2393,103 @@
       </c>
       <c r="H17" s="8"/>
       <c r="I17" s="8">
-        <f t="shared" si="32"/>
+        <f t="shared" ref="I17:I18" si="48">G17-H17</f>
         <v>4</v>
       </c>
       <c r="J17" s="10"/>
       <c r="K17" s="8"/>
       <c r="L17" s="8">
-        <f t="shared" si="33"/>
+        <f t="shared" ref="L17:L18" si="49">I17-K17</f>
         <v>4</v>
       </c>
       <c r="M17" s="10"/>
       <c r="N17" s="8"/>
       <c r="O17" s="8">
-        <f t="shared" si="34"/>
+        <f t="shared" ref="O17:O18" si="50">L17-N17</f>
         <v>4</v>
       </c>
       <c r="P17" s="10"/>
       <c r="Q17" s="8"/>
       <c r="R17" s="8">
-        <f t="shared" si="35"/>
+        <f t="shared" ref="R17:R18" si="51">O17-Q17</f>
         <v>4</v>
       </c>
       <c r="S17" s="10"/>
       <c r="T17" s="8"/>
       <c r="U17" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" ref="U17:U18" si="52">R17-T17</f>
         <v>4</v>
       </c>
       <c r="V17" s="10"/>
       <c r="W17" s="8"/>
       <c r="X17" s="8">
-        <f t="shared" si="37"/>
+        <f t="shared" ref="X17:X18" si="53">U17-W17</f>
         <v>4</v>
       </c>
       <c r="Y17" s="10"/>
       <c r="Z17" s="8"/>
       <c r="AA17" s="8">
-        <f t="shared" si="38"/>
+        <f t="shared" ref="AA17:AA18" si="54">X17-Z17</f>
         <v>4</v>
       </c>
       <c r="AB17" s="10"/>
       <c r="AC17" s="8"/>
       <c r="AD17" s="8">
-        <f t="shared" si="39"/>
+        <f t="shared" ref="AD17:AD18" si="55">AA17-AC17</f>
         <v>4</v>
       </c>
       <c r="AE17" s="10"/>
       <c r="AF17" s="8"/>
       <c r="AG17" s="8">
-        <f t="shared" si="40"/>
+        <f t="shared" ref="AG17:AG18" si="56">AD17-AF17</f>
         <v>4</v>
       </c>
       <c r="AH17" s="10"/>
       <c r="AI17" s="8"/>
       <c r="AJ17" s="8">
-        <f t="shared" si="41"/>
+        <f t="shared" ref="AJ17:AJ18" si="57">AG17-AI17</f>
         <v>4</v>
       </c>
       <c r="AK17" s="10"/>
       <c r="AL17" s="8"/>
       <c r="AM17" s="8">
-        <f t="shared" si="42"/>
+        <f t="shared" ref="AM17:AM18" si="58">AJ17-AL17</f>
         <v>4</v>
       </c>
       <c r="AN17" s="10"/>
       <c r="AO17" s="8"/>
       <c r="AP17" s="8">
-        <f t="shared" si="43"/>
+        <f t="shared" ref="AP17:AP18" si="59">AM17-AO17</f>
         <v>4</v>
       </c>
       <c r="AQ17" s="10"/>
       <c r="AR17" s="8"/>
       <c r="AS17" s="8">
-        <f t="shared" si="44"/>
+        <f t="shared" ref="AS17:AS18" si="60">AP17-AR17</f>
         <v>4</v>
       </c>
       <c r="AT17" s="10"/>
       <c r="AU17" s="8"/>
       <c r="AV17" s="8">
-        <f t="shared" si="45"/>
+        <f t="shared" ref="AV17:AV18" si="61">AS17-AU17</f>
         <v>4</v>
       </c>
       <c r="AW17" s="10"/>
       <c r="AX17" s="8"/>
       <c r="AY17" s="8">
-        <f t="shared" si="46"/>
+        <f t="shared" ref="AY17:AY18" si="62">AV17-AX17</f>
         <v>4</v>
       </c>
       <c r="AZ17" s="15"/>
       <c r="BA17" s="11">
-        <f t="shared" si="47"/>
+        <f t="shared" ref="BA17:BA18" si="63">G17-AZ17</f>
         <v>4</v>
       </c>
     </row>
     <row r="18" spans="2:53" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B18" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="D18" s="5" t="s">
+      <c r="B18" s="13"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="16" t="s">
         <v>78</v>
       </c>
       <c r="E18" s="5" t="s">
@@ -2495,102 +2503,102 @@
       </c>
       <c r="H18" s="8"/>
       <c r="I18" s="8">
-        <f t="shared" si="32"/>
+        <f t="shared" si="48"/>
         <v>4</v>
       </c>
       <c r="J18" s="10"/>
       <c r="K18" s="8"/>
       <c r="L18" s="8">
-        <f t="shared" si="33"/>
+        <f t="shared" si="49"/>
         <v>4</v>
       </c>
       <c r="M18" s="10"/>
       <c r="N18" s="8"/>
       <c r="O18" s="8">
-        <f t="shared" si="34"/>
+        <f t="shared" si="50"/>
         <v>4</v>
       </c>
       <c r="P18" s="10"/>
       <c r="Q18" s="8"/>
       <c r="R18" s="8">
-        <f t="shared" si="35"/>
+        <f t="shared" si="51"/>
         <v>4</v>
       </c>
       <c r="S18" s="10"/>
       <c r="T18" s="8"/>
       <c r="U18" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" si="52"/>
         <v>4</v>
       </c>
       <c r="V18" s="10"/>
       <c r="W18" s="8"/>
       <c r="X18" s="8">
-        <f t="shared" si="37"/>
+        <f t="shared" si="53"/>
         <v>4</v>
       </c>
       <c r="Y18" s="10"/>
       <c r="Z18" s="8"/>
       <c r="AA18" s="8">
-        <f t="shared" si="38"/>
+        <f t="shared" si="54"/>
         <v>4</v>
       </c>
       <c r="AB18" s="10"/>
       <c r="AC18" s="8"/>
       <c r="AD18" s="8">
-        <f t="shared" si="39"/>
+        <f t="shared" si="55"/>
         <v>4</v>
       </c>
       <c r="AE18" s="10"/>
       <c r="AF18" s="8"/>
       <c r="AG18" s="8">
-        <f t="shared" si="40"/>
+        <f t="shared" si="56"/>
         <v>4</v>
       </c>
       <c r="AH18" s="10"/>
       <c r="AI18" s="8"/>
       <c r="AJ18" s="8">
-        <f t="shared" si="41"/>
+        <f t="shared" si="57"/>
         <v>4</v>
       </c>
       <c r="AK18" s="10"/>
       <c r="AL18" s="8"/>
       <c r="AM18" s="8">
-        <f t="shared" si="42"/>
+        <f t="shared" si="58"/>
         <v>4</v>
       </c>
       <c r="AN18" s="10"/>
       <c r="AO18" s="8"/>
       <c r="AP18" s="8">
-        <f t="shared" si="43"/>
+        <f t="shared" si="59"/>
         <v>4</v>
       </c>
       <c r="AQ18" s="10"/>
       <c r="AR18" s="8"/>
       <c r="AS18" s="8">
-        <f t="shared" si="44"/>
+        <f t="shared" si="60"/>
         <v>4</v>
       </c>
       <c r="AT18" s="10"/>
       <c r="AU18" s="8"/>
       <c r="AV18" s="8">
-        <f t="shared" si="45"/>
+        <f t="shared" si="61"/>
         <v>4</v>
       </c>
       <c r="AW18" s="10"/>
       <c r="AX18" s="8"/>
       <c r="AY18" s="8">
-        <f t="shared" si="46"/>
+        <f t="shared" si="62"/>
         <v>4</v>
       </c>
       <c r="AZ18" s="15"/>
       <c r="BA18" s="11">
-        <f t="shared" si="47"/>
+        <f t="shared" si="63"/>
         <v>4</v>
       </c>
     </row>
     <row r="19" spans="2:53" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B19" s="13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>76</v>
@@ -2704,7 +2712,7 @@
     </row>
     <row r="20" spans="2:53" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B20" s="13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>76</v>
@@ -2818,13 +2826,13 @@
     </row>
     <row r="21" spans="2:53" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B21" s="13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>76</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E21" s="5" t="s">
         <v>54</v>
@@ -2931,14 +2939,10 @@
       </c>
     </row>
     <row r="22" spans="2:53" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B22" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>77</v>
+      <c r="B22" s="13"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="16" t="s">
+        <v>78</v>
       </c>
       <c r="E22" s="5" t="s">
         <v>54</v>
@@ -3045,10 +3049,14 @@
       </c>
     </row>
     <row r="23" spans="2:53" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B23" s="13"/>
-      <c r="C23" s="5"/>
+      <c r="B23" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>82</v>
+      </c>
       <c r="D23" s="16" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="E23" s="5" t="s">
         <v>54</v>
@@ -3057,221 +3065,217 @@
         <v>79</v>
       </c>
       <c r="G23" s="5">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="H23" s="8"/>
       <c r="I23" s="8">
-        <f t="shared" si="32"/>
-        <v>4</v>
+        <f t="shared" ref="I23:I25" si="64">G23-H23</f>
+        <v>18</v>
       </c>
       <c r="J23" s="10"/>
       <c r="K23" s="8"/>
       <c r="L23" s="8">
-        <f t="shared" si="33"/>
-        <v>4</v>
+        <f t="shared" ref="L23:L25" si="65">I23-K23</f>
+        <v>18</v>
       </c>
       <c r="M23" s="10"/>
       <c r="N23" s="8"/>
       <c r="O23" s="8">
-        <f t="shared" si="34"/>
-        <v>4</v>
+        <f t="shared" ref="O23:O25" si="66">L23-N23</f>
+        <v>18</v>
       </c>
       <c r="P23" s="10"/>
       <c r="Q23" s="8"/>
       <c r="R23" s="8">
-        <f t="shared" si="35"/>
-        <v>4</v>
+        <f t="shared" ref="R23:R25" si="67">O23-Q23</f>
+        <v>18</v>
       </c>
       <c r="S23" s="10"/>
       <c r="T23" s="8"/>
       <c r="U23" s="8">
-        <f t="shared" si="36"/>
-        <v>4</v>
+        <f t="shared" ref="U23:U25" si="68">R23-T23</f>
+        <v>18</v>
       </c>
       <c r="V23" s="10"/>
       <c r="W23" s="8"/>
       <c r="X23" s="8">
-        <f t="shared" si="37"/>
-        <v>4</v>
+        <f t="shared" ref="X23:X25" si="69">U23-W23</f>
+        <v>18</v>
       </c>
       <c r="Y23" s="10"/>
       <c r="Z23" s="8"/>
       <c r="AA23" s="8">
-        <f t="shared" si="38"/>
-        <v>4</v>
+        <f t="shared" ref="AA23:AA25" si="70">X23-Z23</f>
+        <v>18</v>
       </c>
       <c r="AB23" s="10"/>
       <c r="AC23" s="8"/>
       <c r="AD23" s="8">
-        <f t="shared" si="39"/>
-        <v>4</v>
+        <f t="shared" ref="AD23:AD25" si="71">AA23-AC23</f>
+        <v>18</v>
       </c>
       <c r="AE23" s="10"/>
       <c r="AF23" s="8"/>
       <c r="AG23" s="8">
-        <f t="shared" si="40"/>
-        <v>4</v>
+        <f t="shared" ref="AG23:AG25" si="72">AD23-AF23</f>
+        <v>18</v>
       </c>
       <c r="AH23" s="10"/>
       <c r="AI23" s="8"/>
       <c r="AJ23" s="8">
-        <f t="shared" si="41"/>
-        <v>4</v>
+        <f t="shared" ref="AJ23:AJ25" si="73">AG23-AI23</f>
+        <v>18</v>
       </c>
       <c r="AK23" s="10"/>
       <c r="AL23" s="8"/>
       <c r="AM23" s="8">
-        <f t="shared" si="42"/>
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="AN23" s="10"/>
       <c r="AO23" s="8"/>
       <c r="AP23" s="8">
-        <f t="shared" si="43"/>
-        <v>4</v>
+        <f t="shared" ref="AP23:AP25" si="74">AM23-AO23</f>
+        <v>13</v>
       </c>
       <c r="AQ23" s="10"/>
       <c r="AR23" s="8"/>
       <c r="AS23" s="8">
-        <f t="shared" si="44"/>
-        <v>4</v>
+        <f t="shared" ref="AS23:AS25" si="75">AP23-AR23</f>
+        <v>13</v>
       </c>
       <c r="AT23" s="10"/>
       <c r="AU23" s="8"/>
       <c r="AV23" s="8">
-        <f t="shared" si="45"/>
-        <v>4</v>
+        <f t="shared" ref="AV23:AV25" si="76">AS23-AU23</f>
+        <v>13</v>
       </c>
       <c r="AW23" s="10"/>
       <c r="AX23" s="8"/>
       <c r="AY23" s="8">
-        <f t="shared" si="46"/>
-        <v>4</v>
+        <f t="shared" ref="AY23:AY25" si="77">AV23-AX23</f>
+        <v>13</v>
       </c>
       <c r="AZ23" s="15"/>
       <c r="BA23" s="11">
-        <f t="shared" si="47"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="2:53" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B24" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>82</v>
-      </c>
+        <f t="shared" ref="BA23:BA25" si="78">G23-AZ23</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="2:53" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B24" s="13"/>
+      <c r="C24" s="5"/>
       <c r="D24" s="16" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>54</v>
+        <v>86</v>
       </c>
       <c r="F24" s="5" t="s">
         <v>79</v>
       </c>
       <c r="G24" s="5">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="H24" s="8"/>
       <c r="I24" s="8">
-        <f t="shared" ref="I24:I26" si="48">G24-H24</f>
-        <v>18</v>
+        <f t="shared" si="64"/>
+        <v>10</v>
       </c>
       <c r="J24" s="10"/>
       <c r="K24" s="8"/>
       <c r="L24" s="8">
-        <f t="shared" ref="L24:L26" si="49">I24-K24</f>
-        <v>18</v>
+        <f t="shared" si="65"/>
+        <v>10</v>
       </c>
       <c r="M24" s="10"/>
       <c r="N24" s="8"/>
       <c r="O24" s="8">
-        <f t="shared" ref="O24:O26" si="50">L24-N24</f>
-        <v>18</v>
+        <f t="shared" si="66"/>
+        <v>10</v>
       </c>
       <c r="P24" s="10"/>
       <c r="Q24" s="8"/>
       <c r="R24" s="8">
-        <f t="shared" ref="R24:R26" si="51">O24-Q24</f>
-        <v>18</v>
+        <f t="shared" si="67"/>
+        <v>10</v>
       </c>
       <c r="S24" s="10"/>
       <c r="T24" s="8"/>
       <c r="U24" s="8">
-        <f t="shared" ref="U24:U26" si="52">R24-T24</f>
-        <v>18</v>
+        <f t="shared" si="68"/>
+        <v>10</v>
       </c>
       <c r="V24" s="10"/>
       <c r="W24" s="8"/>
       <c r="X24" s="8">
-        <f t="shared" ref="X24:X26" si="53">U24-W24</f>
-        <v>18</v>
+        <f t="shared" si="69"/>
+        <v>10</v>
       </c>
       <c r="Y24" s="10"/>
       <c r="Z24" s="8"/>
       <c r="AA24" s="8">
-        <f t="shared" ref="AA24:AA26" si="54">X24-Z24</f>
-        <v>18</v>
+        <f t="shared" si="70"/>
+        <v>10</v>
       </c>
       <c r="AB24" s="10"/>
       <c r="AC24" s="8"/>
       <c r="AD24" s="8">
-        <f t="shared" ref="AD24:AD26" si="55">AA24-AC24</f>
-        <v>18</v>
+        <f t="shared" si="71"/>
+        <v>10</v>
       </c>
       <c r="AE24" s="10"/>
       <c r="AF24" s="8"/>
       <c r="AG24" s="8">
-        <f t="shared" ref="AG24:AG26" si="56">AD24-AF24</f>
-        <v>18</v>
+        <f t="shared" si="72"/>
+        <v>10</v>
       </c>
       <c r="AH24" s="10"/>
       <c r="AI24" s="8"/>
       <c r="AJ24" s="8">
-        <f t="shared" ref="AJ24:AJ26" si="57">AG24-AI24</f>
-        <v>18</v>
+        <f t="shared" si="73"/>
+        <v>10</v>
       </c>
       <c r="AK24" s="10"/>
       <c r="AL24" s="8"/>
       <c r="AM24" s="8">
-        <v>13</v>
+        <f t="shared" ref="AM24:AM25" si="79">AJ24-AL24</f>
+        <v>10</v>
       </c>
       <c r="AN24" s="10"/>
       <c r="AO24" s="8"/>
       <c r="AP24" s="8">
-        <f t="shared" ref="AP24:AP26" si="58">AM24-AO24</f>
-        <v>13</v>
+        <f t="shared" si="74"/>
+        <v>10</v>
       </c>
       <c r="AQ24" s="10"/>
       <c r="AR24" s="8"/>
       <c r="AS24" s="8">
-        <f t="shared" ref="AS24:AS26" si="59">AP24-AR24</f>
-        <v>13</v>
+        <f t="shared" si="75"/>
+        <v>10</v>
       </c>
       <c r="AT24" s="10"/>
       <c r="AU24" s="8"/>
       <c r="AV24" s="8">
-        <f t="shared" ref="AV24:AV26" si="60">AS24-AU24</f>
-        <v>13</v>
+        <f t="shared" si="76"/>
+        <v>10</v>
       </c>
       <c r="AW24" s="10"/>
       <c r="AX24" s="8"/>
       <c r="AY24" s="8">
-        <f t="shared" ref="AY24:AY26" si="61">AV24-AX24</f>
-        <v>13</v>
+        <f t="shared" si="77"/>
+        <v>10</v>
       </c>
       <c r="AZ24" s="15"/>
       <c r="BA24" s="11">
-        <f t="shared" ref="BA24:BA26" si="62">G24-AZ24</f>
-        <v>18</v>
+        <f t="shared" si="78"/>
+        <v>10</v>
       </c>
     </row>
     <row r="25" spans="2:53" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B25" s="13"/>
       <c r="C25" s="5"/>
       <c r="D25" s="16" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E25" s="5" t="s">
         <v>86</v>
@@ -3280,215 +3284,110 @@
         <v>79</v>
       </c>
       <c r="G25" s="5">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="H25" s="8"/>
       <c r="I25" s="8">
-        <f t="shared" si="48"/>
-        <v>10</v>
+        <f t="shared" si="64"/>
+        <v>4</v>
       </c>
       <c r="J25" s="10"/>
       <c r="K25" s="8"/>
       <c r="L25" s="8">
-        <f t="shared" si="49"/>
-        <v>10</v>
+        <f t="shared" si="65"/>
+        <v>4</v>
       </c>
       <c r="M25" s="10"/>
       <c r="N25" s="8"/>
       <c r="O25" s="8">
-        <f t="shared" si="50"/>
-        <v>10</v>
+        <f t="shared" si="66"/>
+        <v>4</v>
       </c>
       <c r="P25" s="10"/>
       <c r="Q25" s="8"/>
       <c r="R25" s="8">
-        <f t="shared" si="51"/>
-        <v>10</v>
+        <f t="shared" si="67"/>
+        <v>4</v>
       </c>
       <c r="S25" s="10"/>
       <c r="T25" s="8"/>
       <c r="U25" s="8">
-        <f t="shared" si="52"/>
-        <v>10</v>
+        <f t="shared" si="68"/>
+        <v>4</v>
       </c>
       <c r="V25" s="10"/>
       <c r="W25" s="8"/>
       <c r="X25" s="8">
-        <f t="shared" si="53"/>
-        <v>10</v>
+        <f t="shared" si="69"/>
+        <v>4</v>
       </c>
       <c r="Y25" s="10"/>
       <c r="Z25" s="8"/>
       <c r="AA25" s="8">
-        <f t="shared" si="54"/>
-        <v>10</v>
+        <f t="shared" si="70"/>
+        <v>4</v>
       </c>
       <c r="AB25" s="10"/>
       <c r="AC25" s="8"/>
       <c r="AD25" s="8">
-        <f t="shared" si="55"/>
-        <v>10</v>
+        <f t="shared" si="71"/>
+        <v>4</v>
       </c>
       <c r="AE25" s="10"/>
       <c r="AF25" s="8"/>
       <c r="AG25" s="8">
-        <f t="shared" si="56"/>
-        <v>10</v>
+        <f t="shared" si="72"/>
+        <v>4</v>
       </c>
       <c r="AH25" s="10"/>
       <c r="AI25" s="8"/>
       <c r="AJ25" s="8">
-        <f t="shared" si="57"/>
-        <v>10</v>
+        <f t="shared" si="73"/>
+        <v>4</v>
       </c>
       <c r="AK25" s="10"/>
       <c r="AL25" s="8"/>
       <c r="AM25" s="8">
-        <f t="shared" ref="AM25:AM26" si="63">AJ25-AL25</f>
-        <v>10</v>
+        <f t="shared" si="79"/>
+        <v>4</v>
       </c>
       <c r="AN25" s="10"/>
       <c r="AO25" s="8"/>
       <c r="AP25" s="8">
-        <f t="shared" si="58"/>
-        <v>10</v>
+        <f t="shared" si="74"/>
+        <v>4</v>
       </c>
       <c r="AQ25" s="10"/>
       <c r="AR25" s="8"/>
       <c r="AS25" s="8">
-        <f t="shared" si="59"/>
-        <v>10</v>
+        <f t="shared" si="75"/>
+        <v>4</v>
       </c>
       <c r="AT25" s="10"/>
       <c r="AU25" s="8"/>
       <c r="AV25" s="8">
-        <f t="shared" si="60"/>
-        <v>10</v>
+        <f t="shared" si="76"/>
+        <v>4</v>
       </c>
       <c r="AW25" s="10"/>
       <c r="AX25" s="8"/>
       <c r="AY25" s="8">
-        <f t="shared" si="61"/>
-        <v>10</v>
+        <f t="shared" si="77"/>
+        <v>4</v>
       </c>
       <c r="AZ25" s="15"/>
       <c r="BA25" s="11">
-        <f t="shared" si="62"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="26" spans="2:53" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B26" s="13"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="E26" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="F26" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="G26" s="5">
-        <v>4</v>
-      </c>
-      <c r="H26" s="8"/>
-      <c r="I26" s="8">
-        <f t="shared" si="48"/>
-        <v>4</v>
-      </c>
-      <c r="J26" s="10"/>
-      <c r="K26" s="8"/>
-      <c r="L26" s="8">
-        <f t="shared" si="49"/>
-        <v>4</v>
-      </c>
-      <c r="M26" s="10"/>
-      <c r="N26" s="8"/>
-      <c r="O26" s="8">
-        <f t="shared" si="50"/>
-        <v>4</v>
-      </c>
-      <c r="P26" s="10"/>
-      <c r="Q26" s="8"/>
-      <c r="R26" s="8">
-        <f t="shared" si="51"/>
-        <v>4</v>
-      </c>
-      <c r="S26" s="10"/>
-      <c r="T26" s="8"/>
-      <c r="U26" s="8">
-        <f t="shared" si="52"/>
-        <v>4</v>
-      </c>
-      <c r="V26" s="10"/>
-      <c r="W26" s="8"/>
-      <c r="X26" s="8">
-        <f t="shared" si="53"/>
-        <v>4</v>
-      </c>
-      <c r="Y26" s="10"/>
-      <c r="Z26" s="8"/>
-      <c r="AA26" s="8">
-        <f t="shared" si="54"/>
-        <v>4</v>
-      </c>
-      <c r="AB26" s="10"/>
-      <c r="AC26" s="8"/>
-      <c r="AD26" s="8">
-        <f t="shared" si="55"/>
-        <v>4</v>
-      </c>
-      <c r="AE26" s="10"/>
-      <c r="AF26" s="8"/>
-      <c r="AG26" s="8">
-        <f t="shared" si="56"/>
-        <v>4</v>
-      </c>
-      <c r="AH26" s="10"/>
-      <c r="AI26" s="8"/>
-      <c r="AJ26" s="8">
-        <f t="shared" si="57"/>
-        <v>4</v>
-      </c>
-      <c r="AK26" s="10"/>
-      <c r="AL26" s="8"/>
-      <c r="AM26" s="8">
-        <f t="shared" si="63"/>
-        <v>4</v>
-      </c>
-      <c r="AN26" s="10"/>
-      <c r="AO26" s="8"/>
-      <c r="AP26" s="8">
-        <f t="shared" si="58"/>
-        <v>4</v>
-      </c>
-      <c r="AQ26" s="10"/>
-      <c r="AR26" s="8"/>
-      <c r="AS26" s="8">
-        <f t="shared" si="59"/>
-        <v>4</v>
-      </c>
-      <c r="AT26" s="10"/>
-      <c r="AU26" s="8"/>
-      <c r="AV26" s="8">
-        <f t="shared" si="60"/>
-        <v>4</v>
-      </c>
-      <c r="AW26" s="10"/>
-      <c r="AX26" s="8"/>
-      <c r="AY26" s="8">
-        <f t="shared" si="61"/>
-        <v>4</v>
-      </c>
-      <c r="AZ26" s="15"/>
-      <c r="BA26" s="11">
-        <f t="shared" si="62"/>
+        <f t="shared" si="78"/>
         <v>4</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="AZ4:BA4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AX4:AY4"/>
     <mergeCell ref="AL4:AM4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="K4:L4"/>
@@ -3500,11 +3399,6 @@
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AF4:AG4"/>
     <mergeCell ref="AI4:AJ4"/>
-    <mergeCell ref="AZ4:BA4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AX4:AY4"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.62992125984251968" right="0.62992125984251968" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>

<commit_message>
Agregado de script final tentativo
</commit_message>
<xml_diff>
--- a/Lista de tareas individuales/Lista_Tareas_Revision_3_-_David_Barcenas_Duran.xlsx
+++ b/Lista de tareas individuales/Lista_Tareas_Revision_3_-_David_Barcenas_Duran.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bestr\Desktop\Repositorios\ItaliaPizza-doc\Lista de tareas individuales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6D8219E-9177-46A0-9020-2D0DBEA5AAC7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00418C54-E68A-4A22-B17E-E9E3D9387E0E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14424" yWindow="2760" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3228" yWindow="2436" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Casos de Uso" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="89">
   <si>
     <t>Columna</t>
   </si>
@@ -301,9 +301,6 @@
   </si>
   <si>
     <t>DBD, JAGL, GSC</t>
-  </si>
-  <si>
-    <t>Finalizado</t>
   </si>
   <si>
     <t>Terminado</t>
@@ -845,10 +842,10 @@
   <dimension ref="A1:BA25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane xSplit="6" ySplit="5" topLeftCell="AB6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="5" topLeftCell="G6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A23" sqref="A23:XFD23"/>
+      <selection pane="bottomRight" activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1149,7 +1146,7 @@
         <v>54</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G6" s="5">
         <v>4</v>
@@ -1711,7 +1708,7 @@
         <v>54</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="G11" s="5">
         <v>4</v>
@@ -1923,7 +1920,7 @@
     </row>
     <row r="13" spans="1:53" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B13" s="13" t="s">
         <v>51</v>
@@ -2162,7 +2159,7 @@
         <v>54</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G15" s="5">
         <v>4</v>
@@ -3383,11 +3380,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="AZ4:BA4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AX4:AY4"/>
     <mergeCell ref="AL4:AM4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="K4:L4"/>
@@ -3399,6 +3391,11 @@
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AF4:AG4"/>
     <mergeCell ref="AI4:AJ4"/>
+    <mergeCell ref="AZ4:BA4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AX4:AY4"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.62992125984251968" right="0.62992125984251968" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>

<commit_message>
Actualizacion a lista de tareas David
</commit_message>
<xml_diff>
--- a/Lista de tareas individuales/Lista_Tareas_Revision_3_-_David_Barcenas_Duran.xlsx
+++ b/Lista de tareas individuales/Lista_Tareas_Revision_3_-_David_Barcenas_Duran.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bestr\Desktop\Repositorios\ItaliaPizza-doc\Lista de tareas individuales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00418C54-E68A-4A22-B17E-E9E3D9387E0E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CA35EF5-DF3B-494A-87DA-A434D2E9051F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3228" yWindow="2436" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Casos de Uso" sheetId="1" r:id="rId1"/>
@@ -842,10 +842,10 @@
   <dimension ref="A1:BA25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane xSplit="6" ySplit="5" topLeftCell="G6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="5" topLeftCell="G9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="G9" sqref="G9"/>
+      <selection pane="bottomRight" activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1484,7 +1484,7 @@
         <v>54</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="G9" s="5">
         <v>4</v>
@@ -3380,6 +3380,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="AZ4:BA4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AX4:AY4"/>
     <mergeCell ref="AL4:AM4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="K4:L4"/>
@@ -3391,11 +3396,6 @@
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AF4:AG4"/>
     <mergeCell ref="AI4:AJ4"/>
-    <mergeCell ref="AZ4:BA4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AX4:AY4"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.62992125984251968" right="0.62992125984251968" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>